<commit_message>
City index 25 5/12.
</commit_message>
<xml_diff>
--- a/data_indexpoints_tidy/tallmateriale_19953.xlsx
+++ b/data_indexpoints_tidy/tallmateriale_19953.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Programmering\R\byindeks\data_indexpoints_tidy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F3E197-8129-4A3C-B46F-07CCAD0FE490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5F3EED-B035-41B8-8E2A-3126B776B48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="57600" windowHeight="15345" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="punkt_adt" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="215">
   <si>
     <t>trp_id</t>
   </si>
@@ -383,7 +383,7 @@
     <t>Lundsbrua</t>
   </si>
   <si>
-    <t>FV471 S1D1 m2560</t>
+    <t>FV471 S1D1 m2558</t>
   </si>
   <si>
     <t>0.47077@121488</t>
@@ -395,7 +395,7 @@
     <t>Jernbanen</t>
   </si>
   <si>
-    <t>FV471 S1D1 m4146</t>
+    <t>FV471 S1D1 m4143</t>
   </si>
   <si>
     <t>0.9575@121488</t>
@@ -407,7 +407,7 @@
     <t>Sødal</t>
   </si>
   <si>
-    <t>FV482 S1D1 m2215</t>
+    <t>FV482 S1D1 m2214</t>
   </si>
   <si>
     <t>fv. 482</t>
@@ -464,7 +464,7 @@
     <t>Tinnheiveien</t>
   </si>
   <si>
-    <t>KV18470 S1D1 m310</t>
+    <t>KV18470 S1D1 m309</t>
   </si>
   <si>
     <t>kv. 18470</t>
@@ -479,7 +479,7 @@
     <t>Tretjønnveien</t>
   </si>
   <si>
-    <t>KV18900 S1D1 m3277</t>
+    <t>KV18900 S1D1 m3280</t>
   </si>
   <si>
     <t>kv. 18900</t>
@@ -596,9 +596,6 @@
     <t>2024-2025</t>
   </si>
   <si>
-    <t>jan-nov</t>
-  </si>
-  <si>
     <t>chained</t>
   </si>
   <si>
@@ -663,6 +660,15 @@
   </si>
   <si>
     <t>2023 - (des 2024 - nov 2025)</t>
+  </si>
+  <si>
+    <t>2023 - (jan 2025 - des 2025)</t>
+  </si>
+  <si>
+    <t>2023 - (jan 2024 - des 2025)</t>
+  </si>
+  <si>
+    <t>24_months</t>
   </si>
 </sst>
 </file>
@@ -1023,9 +1029,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1098,10 +1104,10 @@
         <v>22</v>
       </c>
       <c r="G2">
-        <v>58.153961000000002</v>
+        <v>58.153962</v>
       </c>
       <c r="H2">
-        <v>7.9954689999999999</v>
+        <v>7.9954720000000004</v>
       </c>
       <c r="I2" t="s">
         <v>23</v>
@@ -1110,10 +1116,10 @@
         <v>24</v>
       </c>
       <c r="K2">
-        <v>1460</v>
+        <v>1480</v>
       </c>
       <c r="L2">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M2">
         <v>1390</v>
@@ -1125,13 +1131,13 @@
         <v>70</v>
       </c>
       <c r="P2">
-        <v>1800</v>
+        <v>1840</v>
       </c>
       <c r="Q2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1163,10 +1169,10 @@
         <v>24</v>
       </c>
       <c r="K3">
-        <v>1570</v>
+        <v>1600</v>
       </c>
       <c r="L3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M3">
         <v>1490</v>
@@ -1178,13 +1184,13 @@
         <v>100</v>
       </c>
       <c r="P3">
-        <v>1940</v>
+        <v>1990</v>
       </c>
       <c r="Q3">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>58.154001000000001</v>
       </c>
       <c r="H4">
-        <v>7.9954210000000003</v>
+        <v>7.9954219999999996</v>
       </c>
       <c r="I4" t="s">
         <v>32</v>
@@ -1216,10 +1222,10 @@
         <v>24</v>
       </c>
       <c r="K4">
-        <v>21540</v>
+        <v>21490</v>
       </c>
       <c r="L4">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M4">
         <v>21820</v>
@@ -1231,13 +1237,13 @@
         <v>2770</v>
       </c>
       <c r="P4">
-        <v>23710</v>
+        <v>23610</v>
       </c>
       <c r="Q4">
-        <v>2680</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>2670</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1269,10 +1275,10 @@
         <v>24</v>
       </c>
       <c r="K5">
-        <v>21180</v>
+        <v>21200</v>
       </c>
       <c r="L5">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M5">
         <v>21480</v>
@@ -1284,13 +1290,13 @@
         <v>2700</v>
       </c>
       <c r="P5">
-        <v>23080</v>
+        <v>23030</v>
       </c>
       <c r="Q5">
-        <v>2690</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1322,10 +1328,10 @@
         <v>24</v>
       </c>
       <c r="K6">
-        <v>4680</v>
+        <v>4350</v>
       </c>
       <c r="L6">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M6">
         <v>4710</v>
@@ -1337,13 +1343,13 @@
         <v>210</v>
       </c>
       <c r="P6">
-        <v>5410</v>
+        <v>5020</v>
       </c>
       <c r="Q6">
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1363,7 +1369,7 @@
         <v>22</v>
       </c>
       <c r="G7">
-        <v>58.160961</v>
+        <v>58.160961999999998</v>
       </c>
       <c r="H7">
         <v>8.0193729999999999</v>
@@ -1375,10 +1381,10 @@
         <v>24</v>
       </c>
       <c r="K7">
-        <v>4920</v>
+        <v>4560</v>
       </c>
       <c r="L7">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M7">
         <v>5240</v>
@@ -1390,13 +1396,13 @@
         <v>730</v>
       </c>
       <c r="P7">
-        <v>5600</v>
+        <v>5140</v>
       </c>
       <c r="Q7">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1428,10 +1434,10 @@
         <v>24</v>
       </c>
       <c r="K8">
-        <v>5100</v>
+        <v>4600</v>
       </c>
       <c r="L8">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M8">
         <v>5050</v>
@@ -1443,13 +1449,13 @@
         <v>730</v>
       </c>
       <c r="P8">
-        <v>5840</v>
+        <v>5270</v>
       </c>
       <c r="Q8">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1481,10 +1487,10 @@
         <v>24</v>
       </c>
       <c r="K9">
-        <v>3480</v>
+        <v>3990</v>
       </c>
       <c r="L9">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M9">
         <v>4270</v>
@@ -1496,13 +1502,13 @@
         <v>360</v>
       </c>
       <c r="P9">
-        <v>3950</v>
+        <v>4500</v>
       </c>
       <c r="Q9">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1525,7 +1531,7 @@
         <v>58.165139000000003</v>
       </c>
       <c r="H10">
-        <v>8.087548</v>
+        <v>8.0875459999999997</v>
       </c>
       <c r="I10" t="s">
         <v>56</v>
@@ -1534,10 +1540,10 @@
         <v>24</v>
       </c>
       <c r="K10">
-        <v>32110</v>
+        <v>32370</v>
       </c>
       <c r="L10">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M10">
         <v>32070</v>
@@ -1549,13 +1555,13 @@
         <v>4640</v>
       </c>
       <c r="P10">
-        <v>35700</v>
+        <v>35850</v>
       </c>
       <c r="Q10">
-        <v>4450</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>4490</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -1587,10 +1593,10 @@
         <v>24</v>
       </c>
       <c r="K11">
-        <v>22780</v>
+        <v>22810</v>
       </c>
       <c r="L11">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M11">
         <v>23060</v>
@@ -1602,13 +1608,13 @@
         <v>4840</v>
       </c>
       <c r="P11">
-        <v>25100</v>
+        <v>25020</v>
       </c>
       <c r="Q11">
-        <v>4840</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>4690</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -1640,10 +1646,10 @@
         <v>24</v>
       </c>
       <c r="K12">
-        <v>4390</v>
+        <v>2350</v>
       </c>
       <c r="L12">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M12">
         <v>4400</v>
@@ -1655,13 +1661,13 @@
         <v>1070</v>
       </c>
       <c r="P12">
-        <v>4650</v>
+        <v>2520</v>
       </c>
       <c r="Q12">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -1693,10 +1699,10 @@
         <v>24</v>
       </c>
       <c r="K13">
-        <v>4990</v>
+        <v>4980</v>
       </c>
       <c r="L13">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M13">
         <v>5250</v>
@@ -1708,13 +1714,13 @@
         <v>1100</v>
       </c>
       <c r="P13">
-        <v>5440</v>
+        <v>5410</v>
       </c>
       <c r="Q13">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -1746,10 +1752,10 @@
         <v>24</v>
       </c>
       <c r="K14">
-        <v>9160</v>
+        <v>9620</v>
       </c>
       <c r="L14">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M14">
         <v>9950</v>
@@ -1761,13 +1767,13 @@
         <v>1970</v>
       </c>
       <c r="P14">
-        <v>10000</v>
+        <v>10490</v>
       </c>
       <c r="Q14">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -1787,10 +1793,10 @@
         <v>22</v>
       </c>
       <c r="G15">
-        <v>58.178251000000003</v>
+        <v>58.178254000000003</v>
       </c>
       <c r="H15">
-        <v>8.0984309999999997</v>
+        <v>8.0984289999999994</v>
       </c>
       <c r="I15" t="s">
         <v>79</v>
@@ -1799,10 +1805,10 @@
         <v>24</v>
       </c>
       <c r="K15">
-        <v>10770</v>
+        <v>11330</v>
       </c>
       <c r="L15">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M15">
         <v>10750</v>
@@ -1814,13 +1820,13 @@
         <v>1160</v>
       </c>
       <c r="P15">
-        <v>11770</v>
+        <v>12340</v>
       </c>
       <c r="Q15">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1852,10 +1858,10 @@
         <v>24</v>
       </c>
       <c r="K16">
-        <v>2900</v>
+        <v>3000</v>
       </c>
       <c r="L16">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="M16">
         <v>2900</v>
@@ -1867,13 +1873,13 @@
         <v>280</v>
       </c>
       <c r="P16">
-        <v>3090</v>
+        <v>3220</v>
       </c>
       <c r="Q16">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -1905,10 +1911,10 @@
         <v>24</v>
       </c>
       <c r="K17">
-        <v>12030</v>
+        <v>11520</v>
       </c>
       <c r="L17">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M17">
         <v>12250</v>
@@ -1920,13 +1926,13 @@
         <v>830</v>
       </c>
       <c r="P17">
-        <v>13060</v>
+        <v>12430</v>
       </c>
       <c r="Q17">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -1958,10 +1964,10 @@
         <v>24</v>
       </c>
       <c r="K18">
-        <v>9510</v>
+        <v>9590</v>
       </c>
       <c r="L18">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M18">
         <v>9420</v>
@@ -1973,13 +1979,13 @@
         <v>940</v>
       </c>
       <c r="P18">
-        <v>10470</v>
+        <v>10510</v>
       </c>
       <c r="Q18">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>93</v>
       </c>
@@ -2011,10 +2017,10 @@
         <v>24</v>
       </c>
       <c r="K19">
-        <v>10780</v>
+        <v>11040</v>
       </c>
       <c r="L19">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M19">
         <v>10650</v>
@@ -2026,13 +2032,13 @@
         <v>720</v>
       </c>
       <c r="P19">
-        <v>11770</v>
+        <v>11970</v>
       </c>
       <c r="Q19">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -2064,10 +2070,10 @@
         <v>24</v>
       </c>
       <c r="K20">
-        <v>23330</v>
+        <v>22800</v>
       </c>
       <c r="L20">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M20">
         <v>23380</v>
@@ -2079,13 +2085,13 @@
         <v>2220</v>
       </c>
       <c r="P20">
-        <v>25650</v>
+        <v>25040</v>
       </c>
       <c r="Q20">
-        <v>2180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+        <v>2170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -2117,10 +2123,10 @@
         <v>24</v>
       </c>
       <c r="K21">
-        <v>16220</v>
+        <v>16510</v>
       </c>
       <c r="L21">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M21">
         <v>16370</v>
@@ -2132,13 +2138,13 @@
         <v>2090</v>
       </c>
       <c r="P21">
-        <v>17660</v>
+        <v>18040</v>
       </c>
       <c r="Q21">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>107</v>
       </c>
@@ -2191,7 +2197,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>112</v>
       </c>
@@ -2223,10 +2229,10 @@
         <v>24</v>
       </c>
       <c r="K23">
-        <v>6430</v>
+        <v>6420</v>
       </c>
       <c r="L23">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M23">
         <v>6560</v>
@@ -2238,13 +2244,13 @@
         <v>1250</v>
       </c>
       <c r="P23">
-        <v>7620</v>
+        <v>7590</v>
       </c>
       <c r="Q23">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -2267,7 +2273,7 @@
         <v>58.150596999999998</v>
       </c>
       <c r="H24">
-        <v>8.0065530000000003</v>
+        <v>8.0065519999999992</v>
       </c>
       <c r="I24" t="s">
         <v>120</v>
@@ -2276,10 +2282,10 @@
         <v>24</v>
       </c>
       <c r="K24">
-        <v>7780</v>
+        <v>7140</v>
       </c>
       <c r="L24">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M24">
         <v>7600</v>
@@ -2291,13 +2297,13 @@
         <v>1550</v>
       </c>
       <c r="P24">
-        <v>8330</v>
+        <v>7690</v>
       </c>
       <c r="Q24">
-        <v>1620</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>121</v>
       </c>
@@ -2329,10 +2335,10 @@
         <v>24</v>
       </c>
       <c r="K25">
-        <v>15720</v>
+        <v>15150</v>
       </c>
       <c r="L25">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M25">
         <v>16020</v>
@@ -2344,13 +2350,13 @@
         <v>2500</v>
       </c>
       <c r="P25">
-        <v>16610</v>
+        <v>16010</v>
       </c>
       <c r="Q25">
-        <v>2510</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>125</v>
       </c>
@@ -2382,10 +2388,10 @@
         <v>24</v>
       </c>
       <c r="K26">
-        <v>6360</v>
+        <v>6620</v>
       </c>
       <c r="L26">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M26">
         <v>6100</v>
@@ -2397,13 +2403,13 @@
         <v>620</v>
       </c>
       <c r="P26">
-        <v>7020</v>
+        <v>7290</v>
       </c>
       <c r="Q26">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -2423,10 +2429,10 @@
         <v>22</v>
       </c>
       <c r="G27">
-        <v>58.138382</v>
+        <v>58.138381000000003</v>
       </c>
       <c r="H27">
-        <v>8.074738</v>
+        <v>8.0747370000000007</v>
       </c>
       <c r="I27" t="s">
         <v>134</v>
@@ -2435,10 +2441,10 @@
         <v>24</v>
       </c>
       <c r="K27">
-        <v>8600</v>
+        <v>8300</v>
       </c>
       <c r="L27">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M27">
         <v>8840</v>
@@ -2450,13 +2456,13 @@
         <v>830</v>
       </c>
       <c r="P27">
-        <v>9440</v>
+        <v>9100</v>
       </c>
       <c r="Q27">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -2488,10 +2494,10 @@
         <v>24</v>
       </c>
       <c r="K28">
-        <v>8810</v>
+        <v>8420</v>
       </c>
       <c r="L28">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M28">
         <v>8560</v>
@@ -2503,13 +2509,13 @@
         <v>1590</v>
       </c>
       <c r="P28">
-        <v>10740</v>
+        <v>10300</v>
       </c>
       <c r="Q28">
-        <v>1510</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -2541,10 +2547,10 @@
         <v>24</v>
       </c>
       <c r="K29">
-        <v>9270</v>
+        <v>8550</v>
       </c>
       <c r="L29">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M29">
         <v>8950</v>
@@ -2556,13 +2562,13 @@
         <v>1410</v>
       </c>
       <c r="P29">
-        <v>10510</v>
+        <v>9710</v>
       </c>
       <c r="Q29">
-        <v>1460</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>144</v>
       </c>
@@ -2594,10 +2600,10 @@
         <v>24</v>
       </c>
       <c r="K30">
-        <v>6790</v>
+        <v>5310</v>
       </c>
       <c r="L30">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M30">
         <v>7080</v>
@@ -2609,13 +2615,13 @@
         <v>500</v>
       </c>
       <c r="P30">
-        <v>7540</v>
+        <v>5890</v>
       </c>
       <c r="Q30">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>149</v>
       </c>
@@ -2638,7 +2644,7 @@
         <v>58.163941000000001</v>
       </c>
       <c r="H31">
-        <v>8.009798</v>
+        <v>8.0097989999999992</v>
       </c>
       <c r="I31" t="s">
         <v>153</v>
@@ -2647,10 +2653,10 @@
         <v>24</v>
       </c>
       <c r="K31">
-        <v>2280</v>
+        <v>2410</v>
       </c>
       <c r="L31">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M31">
         <v>2300</v>
@@ -2662,13 +2668,13 @@
         <v>350</v>
       </c>
       <c r="P31">
-        <v>2500</v>
+        <v>2630</v>
       </c>
       <c r="Q31">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>154</v>
       </c>
@@ -2700,10 +2706,10 @@
         <v>24</v>
       </c>
       <c r="K32">
-        <v>10760</v>
+        <v>9790</v>
       </c>
       <c r="L32">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M32">
         <v>11010</v>
@@ -2715,7 +2721,7 @@
         <v>800</v>
       </c>
       <c r="P32">
-        <v>12560</v>
+        <v>11450</v>
       </c>
       <c r="Q32">
         <v>800</v>
@@ -2728,13 +2734,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2784,7 +2790,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -2834,7 +2840,7 @@
         <v>-2.34</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -2854,7 +2860,7 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -2904,7 +2910,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -2950,8 +2956,11 @@
       <c r="O5">
         <v>-1.29</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P5">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -3001,7 +3010,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3047,8 +3056,11 @@
       <c r="O7">
         <v>-1.17</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P7">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -3098,7 +3110,7 @@
         <v>4.83</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>140</v>
       </c>
@@ -3144,8 +3156,11 @@
       <c r="O9">
         <v>-11.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P9">
+        <v>-3.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -3183,7 +3198,7 @@
         <v>7.89</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -3217,8 +3232,11 @@
       <c r="O11">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P11">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -3253,7 +3271,7 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -3299,8 +3317,11 @@
       <c r="O13">
         <v>-1.1599999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P13">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -3347,7 +3368,7 @@
         <v>2.34</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>107</v>
       </c>
@@ -3379,7 +3400,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3429,7 +3450,7 @@
         <v>-3.52</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -3475,8 +3496,11 @@
       <c r="O17">
         <v>6.76</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P17">
+        <v>10.26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -3526,7 +3550,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -3572,8 +3596,11 @@
       <c r="O19">
         <v>-0.72</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P19">
+        <v>3.28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -3623,7 +3650,7 @@
         <v>-1.49</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -3652,7 +3679,7 @@
         <v>-1.34</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -3702,7 +3729,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -3746,7 +3773,7 @@
         <v>-1.1299999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -3778,7 +3805,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -3812,8 +3839,11 @@
       <c r="O25">
         <v>-5.13</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>130</v>
       </c>
@@ -3851,7 +3881,7 @@
         <v>-1.1399999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -3894,8 +3924,11 @@
       <c r="O27">
         <v>-1.38</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P27">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>112</v>
       </c>
@@ -3945,7 +3978,7 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -3991,8 +4024,11 @@
       <c r="O29">
         <v>-1.66</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P29">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -4042,7 +4078,7 @@
         <v>2.67</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -4088,13 +4124,16 @@
       <c r="O31">
         <v>3.94</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P31">
+        <v>6.21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
@@ -4102,13 +4141,49 @@
       <c r="D32">
         <v>2024</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E32">
+        <v>-6.55</v>
+      </c>
+      <c r="F32">
+        <v>2.68</v>
+      </c>
+      <c r="G32">
+        <v>-7.95</v>
+      </c>
+      <c r="H32">
+        <v>26.62</v>
+      </c>
+      <c r="I32">
+        <v>11.86</v>
+      </c>
+      <c r="J32">
+        <v>2.92</v>
+      </c>
+      <c r="K32">
+        <v>11.93</v>
+      </c>
+      <c r="L32">
+        <v>6.1</v>
+      </c>
+      <c r="M32">
+        <v>7.86</v>
+      </c>
+      <c r="N32">
+        <v>5.47</v>
+      </c>
+      <c r="O32">
+        <v>-2.77</v>
+      </c>
+      <c r="P32">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
         <v>20</v>
@@ -4116,22 +4191,49 @@
       <c r="D33">
         <v>2025</v>
       </c>
+      <c r="E33">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="F33">
+        <v>1.54</v>
+      </c>
+      <c r="G33">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="H33">
+        <v>-8.64</v>
+      </c>
+      <c r="I33">
+        <v>-0.65</v>
+      </c>
+      <c r="J33">
+        <v>1.27</v>
+      </c>
       <c r="K33">
-        <v>-5.66</v>
+        <v>2.31</v>
       </c>
       <c r="L33">
-        <v>-9.4</v>
+        <v>1.45</v>
       </c>
       <c r="M33">
-        <v>-10.46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+        <v>2.62</v>
+      </c>
+      <c r="N33">
+        <v>5.28</v>
+      </c>
+      <c r="O33">
+        <v>2.59</v>
+      </c>
+      <c r="P33">
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
         <v>20</v>
@@ -4140,48 +4242,48 @@
         <v>2024</v>
       </c>
       <c r="E34">
-        <v>-6.55</v>
+        <v>-5.16</v>
       </c>
       <c r="F34">
-        <v>2.68</v>
+        <v>1.55</v>
       </c>
       <c r="G34">
-        <v>-7.95</v>
+        <v>-10.6</v>
       </c>
       <c r="H34">
-        <v>26.62</v>
+        <v>20.03</v>
       </c>
       <c r="I34">
-        <v>11.86</v>
+        <v>2.09</v>
       </c>
       <c r="J34">
-        <v>2.92</v>
+        <v>-2.9</v>
       </c>
       <c r="K34">
-        <v>11.93</v>
+        <v>0.25</v>
       </c>
       <c r="L34">
-        <v>6.1</v>
+        <v>-2.83</v>
       </c>
       <c r="M34">
-        <v>7.86</v>
+        <v>-4.2</v>
       </c>
       <c r="N34">
-        <v>5.47</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="O34">
-        <v>-2.77</v>
+        <v>-4.55</v>
       </c>
       <c r="P34">
-        <v>4.88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-0.54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
         <v>20</v>
@@ -4189,46 +4291,13 @@
       <c r="D35">
         <v>2025</v>
       </c>
-      <c r="E35">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="F35">
-        <v>1.54</v>
-      </c>
-      <c r="G35">
-        <v>10.119999999999999</v>
-      </c>
-      <c r="H35">
-        <v>-8.64</v>
-      </c>
-      <c r="I35">
-        <v>-0.65</v>
-      </c>
-      <c r="J35">
-        <v>1.27</v>
-      </c>
-      <c r="K35">
-        <v>2.31</v>
-      </c>
-      <c r="L35">
-        <v>1.45</v>
-      </c>
-      <c r="M35">
-        <v>2.62</v>
-      </c>
-      <c r="N35">
-        <v>5.28</v>
-      </c>
-      <c r="O35">
-        <v>2.59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C36" t="s">
         <v>20</v>
@@ -4237,48 +4306,48 @@
         <v>2024</v>
       </c>
       <c r="E36">
-        <v>-5.16</v>
+        <v>-11.49</v>
       </c>
       <c r="F36">
-        <v>1.55</v>
+        <v>-3.28</v>
       </c>
       <c r="G36">
-        <v>-10.6</v>
+        <v>-11.08</v>
       </c>
       <c r="H36">
-        <v>20.03</v>
+        <v>17.02</v>
       </c>
       <c r="I36">
-        <v>2.09</v>
+        <v>-0.77</v>
       </c>
       <c r="J36">
-        <v>-2.9</v>
+        <v>-2</v>
       </c>
       <c r="K36">
-        <v>0.25</v>
+        <v>5.53</v>
       </c>
       <c r="L36">
-        <v>-2.83</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="M36">
-        <v>-4.2</v>
+        <v>14.75</v>
       </c>
       <c r="N36">
-        <v>0.14000000000000001</v>
+        <v>3.86</v>
       </c>
       <c r="O36">
-        <v>-4.55</v>
+        <v>-1.76</v>
       </c>
       <c r="P36">
-        <v>-0.54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-2.39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C37" t="s">
         <v>20</v>
@@ -4286,977 +4355,909 @@
       <c r="D37">
         <v>2025</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <v>11.43</v>
+      </c>
+      <c r="H37">
+        <v>-10.5</v>
+      </c>
+      <c r="I37">
+        <v>4.3</v>
+      </c>
+      <c r="J37">
+        <v>2.83</v>
+      </c>
+      <c r="K37">
+        <v>2.38</v>
+      </c>
+      <c r="P37">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>157</v>
       </c>
       <c r="D38">
         <v>2024</v>
       </c>
       <c r="E38">
-        <v>-11.49</v>
+        <v>-7.94</v>
       </c>
       <c r="F38">
-        <v>-3.28</v>
-      </c>
-      <c r="G38">
-        <v>-11.08</v>
-      </c>
-      <c r="H38">
-        <v>17.02</v>
+        <v>-3.64</v>
       </c>
       <c r="I38">
-        <v>-0.77</v>
+        <v>-22.19</v>
       </c>
       <c r="J38">
-        <v>-2</v>
+        <v>-14.26</v>
       </c>
       <c r="K38">
-        <v>5.53</v>
+        <v>-0.4</v>
       </c>
       <c r="L38">
-        <v>4.3499999999999996</v>
+        <v>4.17</v>
       </c>
       <c r="M38">
-        <v>14.75</v>
+        <v>-3.03</v>
       </c>
       <c r="N38">
-        <v>3.86</v>
+        <v>6.82</v>
       </c>
       <c r="O38">
-        <v>-1.76</v>
+        <v>3.66</v>
       </c>
       <c r="P38">
-        <v>-2.39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-1.58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="C39" t="s">
-        <v>20</v>
+        <v>157</v>
       </c>
       <c r="D39">
         <v>2025</v>
       </c>
+      <c r="E39">
+        <v>7.88</v>
+      </c>
+      <c r="F39">
+        <v>-7.78</v>
+      </c>
       <c r="G39">
-        <v>11.43</v>
+        <v>-9.42</v>
       </c>
       <c r="H39">
-        <v>-10.5</v>
+        <v>-20.76</v>
       </c>
       <c r="I39">
-        <v>4.3</v>
+        <v>9.68</v>
       </c>
       <c r="J39">
-        <v>2.83</v>
-      </c>
-      <c r="K39">
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-1.78</v>
+      </c>
+      <c r="L39">
+        <v>-15.66</v>
+      </c>
+      <c r="M39">
+        <v>-6.71</v>
+      </c>
+      <c r="N39">
+        <v>-10.88</v>
+      </c>
+      <c r="O39">
+        <v>-12.52</v>
+      </c>
+      <c r="P39">
+        <v>-6.55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C40" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="D40">
         <v>2024</v>
       </c>
       <c r="E40">
-        <v>-7.94</v>
+        <v>-3.33</v>
       </c>
       <c r="F40">
-        <v>-3.64</v>
+        <v>2.92</v>
+      </c>
+      <c r="G40">
+        <v>-6.38</v>
+      </c>
+      <c r="H40">
+        <v>19.78</v>
       </c>
       <c r="I40">
-        <v>-22.19</v>
+        <v>7.11</v>
       </c>
       <c r="J40">
-        <v>-14.26</v>
+        <v>0.71</v>
       </c>
       <c r="K40">
-        <v>-0.4</v>
+        <v>5.17</v>
       </c>
       <c r="L40">
-        <v>4.17</v>
+        <v>4.62</v>
       </c>
       <c r="M40">
-        <v>-3.03</v>
+        <v>1.08</v>
       </c>
       <c r="N40">
-        <v>6.82</v>
+        <v>1.85</v>
       </c>
       <c r="O40">
-        <v>3.66</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="P40">
-        <v>-1.58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B41" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C41" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="D41">
         <v>2025</v>
       </c>
       <c r="E41">
-        <v>7.88</v>
+        <v>6.43</v>
       </c>
       <c r="F41">
-        <v>-7.78</v>
+        <v>-2.52</v>
       </c>
       <c r="G41">
-        <v>-9.42</v>
+        <v>2.46</v>
       </c>
       <c r="H41">
-        <v>-20.76</v>
+        <v>-13.43</v>
       </c>
       <c r="I41">
-        <v>9.68</v>
+        <v>-4.41</v>
       </c>
       <c r="J41">
-        <v>-1.78</v>
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="K41">
+        <v>-4.82</v>
       </c>
       <c r="L41">
-        <v>-15.66</v>
+        <v>-8.76</v>
       </c>
       <c r="M41">
-        <v>-6.71</v>
+        <v>-1.73</v>
       </c>
       <c r="N41">
-        <v>-10.88</v>
+        <v>-5.73</v>
       </c>
       <c r="O41">
-        <v>-12.52</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-6.72</v>
+      </c>
+      <c r="P41">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>138</v>
+        <v>83</v>
       </c>
       <c r="D42">
         <v>2024</v>
       </c>
       <c r="E42">
-        <v>-3.33</v>
+        <v>-11.46</v>
       </c>
       <c r="F42">
-        <v>2.92</v>
+        <v>-5.48</v>
       </c>
       <c r="G42">
-        <v>-6.38</v>
+        <v>-9.52</v>
       </c>
       <c r="H42">
-        <v>19.78</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="I42">
-        <v>7.11</v>
+        <v>-4.7</v>
       </c>
       <c r="J42">
-        <v>0.71</v>
-      </c>
-      <c r="K42">
-        <v>5.17</v>
+        <v>-5.99</v>
       </c>
       <c r="L42">
-        <v>4.62</v>
+        <v>-3.17</v>
       </c>
       <c r="M42">
-        <v>1.08</v>
-      </c>
-      <c r="N42">
-        <v>1.85</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="O42">
-        <v>0.28000000000000003</v>
+        <v>-5.72</v>
       </c>
       <c r="P42">
-        <v>2.17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
+        <v>83</v>
       </c>
       <c r="D43">
         <v>2025</v>
       </c>
       <c r="E43">
+        <v>6.08</v>
+      </c>
+      <c r="F43">
+        <v>-0.7</v>
+      </c>
+      <c r="G43">
         <v>6.43</v>
       </c>
-      <c r="F43">
-        <v>-2.52</v>
-      </c>
-      <c r="G43">
-        <v>2.46</v>
-      </c>
       <c r="H43">
-        <v>-13.43</v>
+        <v>-13.53</v>
       </c>
       <c r="I43">
-        <v>-4.41</v>
+        <v>-3.86</v>
       </c>
       <c r="J43">
-        <v>-10.199999999999999</v>
+        <v>-12</v>
       </c>
       <c r="K43">
-        <v>-4.82</v>
+        <v>-5.22</v>
       </c>
       <c r="L43">
-        <v>-8.76</v>
-      </c>
-      <c r="M43">
-        <v>-1.73</v>
-      </c>
-      <c r="N43">
-        <v>-5.73</v>
+        <v>-1.31</v>
       </c>
       <c r="O43">
-        <v>-6.72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="P43">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="C44" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="D44">
         <v>2024</v>
       </c>
       <c r="E44">
-        <v>-11.46</v>
+        <v>-0.86</v>
       </c>
       <c r="F44">
-        <v>-5.48</v>
+        <v>4.62</v>
       </c>
       <c r="G44">
-        <v>-9.52</v>
+        <v>-2.66</v>
       </c>
       <c r="H44">
-        <v>5.1100000000000003</v>
+        <v>14.5</v>
       </c>
       <c r="I44">
-        <v>-4.7</v>
+        <v>5.56</v>
       </c>
       <c r="J44">
-        <v>-5.99</v>
+        <v>1.57</v>
+      </c>
+      <c r="K44">
+        <v>8.56</v>
       </c>
       <c r="L44">
-        <v>-3.17</v>
+        <v>4.2699999999999996</v>
       </c>
       <c r="M44">
-        <v>-4.4000000000000004</v>
+        <v>2.78</v>
+      </c>
+      <c r="N44">
+        <v>6.32</v>
       </c>
       <c r="O44">
-        <v>-5.72</v>
+        <v>2.97</v>
       </c>
       <c r="P44">
-        <v>-0.45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="C45" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="D45">
         <v>2025</v>
       </c>
       <c r="E45">
+        <v>6.15</v>
+      </c>
+      <c r="F45">
+        <v>1.95</v>
+      </c>
+      <c r="G45">
+        <v>6.58</v>
+      </c>
+      <c r="H45">
+        <v>-2.04</v>
+      </c>
+      <c r="I45">
+        <v>2.74</v>
+      </c>
+      <c r="J45">
+        <v>1.97</v>
+      </c>
+      <c r="K45">
+        <v>3.25</v>
+      </c>
+      <c r="L45">
+        <v>5.68</v>
+      </c>
+      <c r="M45">
+        <v>6.53</v>
+      </c>
+      <c r="N45">
+        <v>5.74</v>
+      </c>
+      <c r="O45">
+        <v>2.96</v>
+      </c>
+      <c r="P45">
         <v>6.08</v>
       </c>
-      <c r="F45">
-        <v>-0.7</v>
-      </c>
-      <c r="G45">
-        <v>6.43</v>
-      </c>
-      <c r="H45">
-        <v>-13.53</v>
-      </c>
-      <c r="I45">
-        <v>-3.86</v>
-      </c>
-      <c r="J45">
-        <v>-12</v>
-      </c>
-      <c r="K45">
-        <v>-5.22</v>
-      </c>
-      <c r="L45">
-        <v>-1.31</v>
-      </c>
-      <c r="O45">
-        <v>4.2699999999999996</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="C46" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="D46">
         <v>2024</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E46">
+        <v>-15.79</v>
+      </c>
+      <c r="F46">
+        <v>-8.9600000000000009</v>
+      </c>
+      <c r="G46">
+        <v>-12.86</v>
+      </c>
+      <c r="H46">
+        <v>3.71</v>
+      </c>
+      <c r="I46">
+        <v>-5.38</v>
+      </c>
+      <c r="J46">
+        <v>-6.19</v>
+      </c>
+      <c r="L46">
+        <v>-2.2400000000000002</v>
+      </c>
+      <c r="M46">
+        <v>1.96</v>
+      </c>
+      <c r="N46">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="O46">
+        <v>7.4</v>
+      </c>
+      <c r="P46">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="D47">
         <v>2025</v>
       </c>
-      <c r="O47">
-        <v>3.82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="D48">
         <v>2024</v>
       </c>
       <c r="E48">
-        <v>-0.86</v>
+        <v>-7.92</v>
       </c>
       <c r="F48">
-        <v>4.62</v>
+        <v>-4.58</v>
       </c>
       <c r="G48">
-        <v>-2.66</v>
+        <v>-11.73</v>
       </c>
       <c r="H48">
-        <v>14.5</v>
+        <v>15.28</v>
       </c>
       <c r="I48">
-        <v>5.56</v>
+        <v>-1.94</v>
       </c>
       <c r="J48">
-        <v>1.57</v>
+        <v>-2.5</v>
       </c>
       <c r="K48">
-        <v>8.56</v>
+        <v>0.41</v>
       </c>
       <c r="L48">
-        <v>4.2699999999999996</v>
-      </c>
-      <c r="M48">
-        <v>2.78</v>
-      </c>
-      <c r="N48">
-        <v>6.32</v>
+        <v>1.07</v>
       </c>
       <c r="O48">
-        <v>2.97</v>
+        <v>-2.02</v>
       </c>
       <c r="P48">
-        <v>1.84</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="D49">
         <v>2025</v>
       </c>
       <c r="E49">
-        <v>6.15</v>
+        <v>6.25</v>
       </c>
       <c r="F49">
-        <v>1.95</v>
+        <v>5.52</v>
       </c>
       <c r="G49">
-        <v>6.58</v>
+        <v>16.93</v>
       </c>
       <c r="H49">
-        <v>-2.04</v>
+        <v>-7.42</v>
       </c>
       <c r="I49">
-        <v>2.74</v>
+        <v>7.78</v>
       </c>
       <c r="J49">
-        <v>1.97</v>
+        <v>9.61</v>
       </c>
       <c r="K49">
-        <v>3.25</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="L49">
-        <v>5.68</v>
-      </c>
-      <c r="M49">
-        <v>6.53</v>
-      </c>
-      <c r="N49">
-        <v>5.74</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="O49">
-        <v>2.96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-0.53</v>
+      </c>
+      <c r="P49">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>66</v>
       </c>
       <c r="B50" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="C50" t="s">
-        <v>147</v>
+        <v>60</v>
       </c>
       <c r="D50">
         <v>2024</v>
       </c>
       <c r="E50">
-        <v>-15.79</v>
+        <v>-12.02</v>
       </c>
       <c r="F50">
-        <v>-8.9600000000000009</v>
+        <v>-6.4</v>
       </c>
       <c r="G50">
-        <v>-12.86</v>
+        <v>-15.41</v>
       </c>
       <c r="H50">
-        <v>3.71</v>
+        <v>2.37</v>
       </c>
       <c r="I50">
-        <v>-5.38</v>
+        <v>-4.2300000000000004</v>
       </c>
       <c r="J50">
-        <v>-6.19</v>
+        <v>-5.95</v>
+      </c>
+      <c r="K50">
+        <v>-4.5599999999999996</v>
       </c>
       <c r="L50">
-        <v>-2.2400000000000002</v>
+        <v>-7.67</v>
       </c>
       <c r="M50">
-        <v>1.96</v>
+        <v>-2.5099999999999998</v>
       </c>
       <c r="N50">
-        <v>9.9700000000000006</v>
+        <v>-0.17</v>
       </c>
       <c r="O50">
-        <v>7.4</v>
+        <v>-3.24</v>
       </c>
       <c r="P50">
-        <v>4.24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-1.49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>60</v>
       </c>
       <c r="D51">
         <v>2025</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="C52" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="D52">
         <v>2024</v>
       </c>
       <c r="E52">
-        <v>-7.92</v>
+        <v>-8.6</v>
       </c>
       <c r="F52">
-        <v>-4.58</v>
+        <v>-1.27</v>
       </c>
       <c r="G52">
-        <v>-11.73</v>
+        <v>-7.22</v>
       </c>
       <c r="H52">
-        <v>15.28</v>
+        <v>13.26</v>
       </c>
       <c r="I52">
-        <v>-1.94</v>
+        <v>2.57</v>
       </c>
       <c r="J52">
-        <v>-2.5</v>
+        <v>0.86</v>
       </c>
       <c r="K52">
-        <v>0.41</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="L52">
-        <v>1.07</v>
+        <v>-0.51</v>
+      </c>
+      <c r="N52">
+        <v>3.53</v>
       </c>
       <c r="O52">
-        <v>-2.02</v>
+        <v>2.87</v>
       </c>
       <c r="P52">
-        <v>4.09</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="D53">
         <v>2025</v>
       </c>
       <c r="E53">
-        <v>6.25</v>
+        <v>8.59</v>
       </c>
       <c r="F53">
-        <v>5.52</v>
+        <v>2.09</v>
       </c>
       <c r="G53">
-        <v>16.93</v>
+        <v>9.69</v>
       </c>
       <c r="H53">
-        <v>-7.42</v>
+        <v>-2.63</v>
       </c>
       <c r="I53">
-        <v>7.78</v>
+        <v>2.19</v>
       </c>
       <c r="J53">
-        <v>9.61</v>
+        <v>0.35</v>
       </c>
       <c r="K53">
-        <v>2.0499999999999998</v>
+        <v>2.42</v>
       </c>
       <c r="L53">
-        <v>5.0999999999999996</v>
+        <v>2.73</v>
+      </c>
+      <c r="N53">
+        <v>2.68</v>
       </c>
       <c r="O53">
-        <v>-0.53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-0.79</v>
+      </c>
+      <c r="P53">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="C54" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="D54">
         <v>2024</v>
       </c>
       <c r="E54">
-        <v>-12.02</v>
+        <v>-7.6</v>
       </c>
       <c r="F54">
-        <v>-6.4</v>
+        <v>-0.4</v>
       </c>
       <c r="G54">
-        <v>-15.41</v>
+        <v>-6.62</v>
       </c>
       <c r="H54">
-        <v>2.37</v>
+        <v>10.86</v>
       </c>
       <c r="I54">
-        <v>-4.2300000000000004</v>
+        <v>1.55</v>
       </c>
       <c r="J54">
-        <v>-5.95</v>
+        <v>-1.43</v>
       </c>
       <c r="K54">
-        <v>-4.5599999999999996</v>
+        <v>1.06</v>
       </c>
       <c r="L54">
-        <v>-7.67</v>
+        <v>-0.9</v>
       </c>
       <c r="M54">
-        <v>-2.5099999999999998</v>
+        <v>-0.85</v>
       </c>
       <c r="N54">
-        <v>-0.17</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="O54">
-        <v>-3.24</v>
+        <v>-0.39</v>
       </c>
       <c r="P54">
-        <v>-1.49</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="C55" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="D55">
         <v>2025</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E55">
+        <v>4.54</v>
+      </c>
+      <c r="F55">
+        <v>-1.6</v>
+      </c>
+      <c r="G55">
+        <v>2.54</v>
+      </c>
+      <c r="H55">
+        <v>-9.0500000000000007</v>
+      </c>
+      <c r="I55">
+        <v>-3.09</v>
+      </c>
+      <c r="J55">
+        <v>-3.97</v>
+      </c>
+      <c r="K55">
+        <v>-1.17</v>
+      </c>
+      <c r="L55">
+        <v>-2.73</v>
+      </c>
+      <c r="M55">
+        <v>-3.76</v>
+      </c>
+      <c r="N55">
+        <v>-2.27</v>
+      </c>
+      <c r="O55">
+        <v>-4.05</v>
+      </c>
+      <c r="P55">
+        <v>-0.47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C56" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D56">
         <v>2024</v>
       </c>
       <c r="E56">
-        <v>-8.6</v>
+        <v>-8.48</v>
       </c>
       <c r="F56">
-        <v>-1.27</v>
+        <v>-3.22</v>
       </c>
       <c r="G56">
-        <v>-7.22</v>
+        <v>-6.6</v>
       </c>
       <c r="H56">
-        <v>13.26</v>
+        <v>9.5</v>
       </c>
       <c r="I56">
-        <v>2.57</v>
+        <v>3.33</v>
       </c>
       <c r="J56">
+        <v>-1.72</v>
+      </c>
+      <c r="K56">
+        <v>1.93</v>
+      </c>
+      <c r="L56">
+        <v>1.65</v>
+      </c>
+      <c r="M56">
         <v>0.86</v>
       </c>
-      <c r="K56">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="L56">
-        <v>-0.51</v>
-      </c>
       <c r="N56">
-        <v>3.53</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="O56">
-        <v>2.87</v>
+        <v>5.08</v>
       </c>
       <c r="P56">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C57" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D57">
         <v>2025</v>
       </c>
       <c r="E57">
-        <v>8.59</v>
+        <v>10.14</v>
       </c>
       <c r="F57">
-        <v>2.09</v>
+        <v>3.9</v>
       </c>
       <c r="G57">
-        <v>9.69</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="H57">
-        <v>-2.63</v>
+        <v>-4.6900000000000004</v>
       </c>
       <c r="I57">
-        <v>2.19</v>
+        <v>-1.53</v>
       </c>
       <c r="J57">
-        <v>0.35</v>
+        <v>-1.59</v>
       </c>
       <c r="K57">
-        <v>2.42</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="L57">
-        <v>2.73</v>
+        <v>-1.19</v>
+      </c>
+      <c r="M57">
+        <v>-1.02</v>
       </c>
       <c r="N57">
-        <v>2.68</v>
+        <v>-0.96</v>
       </c>
       <c r="O57">
-        <v>-0.79</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>98</v>
-      </c>
-      <c r="B58" t="s">
-        <v>99</v>
-      </c>
-      <c r="C58" t="s">
-        <v>101</v>
-      </c>
-      <c r="D58">
-        <v>2024</v>
-      </c>
-      <c r="E58">
-        <v>-7.6</v>
-      </c>
-      <c r="F58">
-        <v>-0.4</v>
-      </c>
-      <c r="G58">
-        <v>-6.62</v>
-      </c>
-      <c r="H58">
-        <v>10.86</v>
-      </c>
-      <c r="I58">
-        <v>1.55</v>
-      </c>
-      <c r="J58">
-        <v>-1.43</v>
-      </c>
-      <c r="K58">
-        <v>1.06</v>
-      </c>
-      <c r="L58">
-        <v>-0.9</v>
-      </c>
-      <c r="M58">
-        <v>-0.85</v>
-      </c>
-      <c r="N58">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="O58">
-        <v>-0.39</v>
-      </c>
-      <c r="P58">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>98</v>
-      </c>
-      <c r="B59" t="s">
-        <v>99</v>
-      </c>
-      <c r="C59" t="s">
-        <v>101</v>
-      </c>
-      <c r="D59">
-        <v>2025</v>
-      </c>
-      <c r="E59">
-        <v>4.54</v>
-      </c>
-      <c r="F59">
-        <v>-1.6</v>
-      </c>
-      <c r="G59">
-        <v>2.54</v>
-      </c>
-      <c r="H59">
-        <v>-9.0500000000000007</v>
-      </c>
-      <c r="I59">
-        <v>-3.09</v>
-      </c>
-      <c r="J59">
-        <v>-3.97</v>
-      </c>
-      <c r="K59">
-        <v>-1.17</v>
-      </c>
-      <c r="L59">
-        <v>-2.73</v>
-      </c>
-      <c r="M59">
-        <v>-3.76</v>
-      </c>
-      <c r="N59">
-        <v>-2.27</v>
-      </c>
-      <c r="O59">
-        <v>-4.05</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B60" t="s">
-        <v>90</v>
-      </c>
-      <c r="C60" t="s">
-        <v>83</v>
-      </c>
-      <c r="D60">
-        <v>2024</v>
-      </c>
-      <c r="E60">
-        <v>-8.48</v>
-      </c>
-      <c r="F60">
-        <v>-3.22</v>
-      </c>
-      <c r="G60">
-        <v>-6.6</v>
-      </c>
-      <c r="H60">
-        <v>9.5</v>
-      </c>
-      <c r="I60">
-        <v>3.33</v>
-      </c>
-      <c r="J60">
-        <v>-1.72</v>
-      </c>
-      <c r="K60">
-        <v>1.93</v>
-      </c>
-      <c r="L60">
-        <v>1.65</v>
-      </c>
-      <c r="M60">
-        <v>0.86</v>
-      </c>
-      <c r="N60">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="O60">
-        <v>5.08</v>
-      </c>
-      <c r="P60">
-        <v>4.29</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>89</v>
-      </c>
-      <c r="B61" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61" t="s">
-        <v>83</v>
-      </c>
-      <c r="D61">
-        <v>2025</v>
-      </c>
-      <c r="E61">
-        <v>10.14</v>
-      </c>
-      <c r="F61">
-        <v>3.9</v>
-      </c>
-      <c r="G61">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="H61">
-        <v>-4.6900000000000004</v>
-      </c>
-      <c r="I61">
-        <v>-1.53</v>
-      </c>
-      <c r="J61">
-        <v>-1.59</v>
-      </c>
-      <c r="K61">
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="L61">
-        <v>-1.19</v>
-      </c>
-      <c r="M61">
-        <v>-1.02</v>
-      </c>
-      <c r="N61">
-        <v>-0.96</v>
-      </c>
-      <c r="O61">
         <v>-2.38</v>
+      </c>
+      <c r="P57">
+        <v>2.75</v>
       </c>
     </row>
   </sheetData>
@@ -5266,13 +5267,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>172</v>
       </c>
@@ -5316,7 +5317,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -5360,7 +5361,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -5368,19 +5369,19 @@
         <v>2025</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>-0.7</v>
+        <v>-0.5</v>
       </c>
       <c r="E3">
-        <v>0.99299999999999999</v>
+        <v>0.99529999999999996</v>
       </c>
       <c r="F3">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3">
-        <v>0.88029622821928633</v>
+        <v>0.8537938585908158</v>
       </c>
       <c r="H3" t="s">
         <v>185</v>
@@ -5392,16 +5393,60 @@
         <v>187</v>
       </c>
       <c r="K3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L3" t="s">
+        <v>188</v>
+      </c>
+      <c r="M3">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="N3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2023</v>
+      </c>
+      <c r="B4">
+        <v>2025</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.98922866999999992</v>
+      </c>
+      <c r="F4">
+        <v>28</v>
+      </c>
+      <c r="G4">
+        <v>1.0441536283273569</v>
+      </c>
+      <c r="H4" t="s">
         <v>190</v>
       </c>
-      <c r="M3">
-        <v>-2.4</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
+      <c r="I4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J4" t="s">
+        <v>187</v>
+      </c>
+      <c r="K4" t="s">
+        <v>171</v>
+      </c>
+      <c r="L4" t="s">
+        <v>188</v>
+      </c>
+      <c r="M4">
+        <v>-3.1</v>
+      </c>
+      <c r="N4">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -5415,9 +5460,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>172</v>
       </c>
@@ -5461,7 +5506,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -5469,19 +5514,19 @@
         <v>2024</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>-0.8</v>
+        <v>-0.6</v>
       </c>
       <c r="E2">
-        <v>0.99180000000000001</v>
+        <v>0.99390000000000001</v>
       </c>
       <c r="F2">
         <v>28</v>
       </c>
       <c r="G2">
-        <v>0.63313349212119308</v>
+        <v>0.61125752998503569</v>
       </c>
       <c r="H2" t="s">
         <v>185</v>
@@ -5493,19 +5538,19 @@
         <v>187</v>
       </c>
       <c r="K2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M2">
-        <v>-2</v>
+        <v>-1.8</v>
       </c>
       <c r="N2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -5513,19 +5558,19 @@
         <v>2025</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>-0.7</v>
+        <v>-0.5</v>
       </c>
       <c r="E3">
-        <v>0.99299999999999999</v>
+        <v>0.99529999999999996</v>
       </c>
       <c r="F3">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3">
-        <v>0.88029622821928633</v>
+        <v>0.8537938585908158</v>
       </c>
       <c r="H3" t="s">
         <v>185</v>
@@ -5537,19 +5582,19 @@
         <v>187</v>
       </c>
       <c r="K3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M3">
-        <v>-2.4</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="N3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2023</v>
       </c>
@@ -5557,40 +5602,40 @@
         <v>2025</v>
       </c>
       <c r="C4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>-1.5</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="E4">
-        <v>0.98485739999999999</v>
+        <v>0.98922866999999992</v>
       </c>
       <c r="F4">
         <v>28</v>
       </c>
       <c r="G4">
-        <v>1.0759003463784551</v>
+        <v>1.0441536283273569</v>
       </c>
       <c r="H4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I4" t="s">
         <v>191</v>
-      </c>
-      <c r="I4" t="s">
-        <v>192</v>
       </c>
       <c r="J4" t="s">
         <v>187</v>
       </c>
       <c r="K4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M4">
-        <v>-3.6</v>
+        <v>-3.1</v>
       </c>
       <c r="N4">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -5600,16 +5645,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="20.7265625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>175</v>
       </c>
@@ -5620,13 +5665,13 @@
         <v>176</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>183</v>
@@ -5635,22 +5680,22 @@
         <v>184</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>159</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.99167141583069263</v>
       </c>
@@ -5676,7 +5721,7 @@
         <v>0.5</v>
       </c>
       <c r="I2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J2" s="2">
         <v>45627</v>
@@ -5688,10 +5733,10 @@
         <v>2024</v>
       </c>
       <c r="M2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.99717957176137251</v>
       </c>
@@ -5717,7 +5762,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J3" s="2">
         <v>45658</v>
@@ -5729,10 +5774,10 @@
         <v>2025</v>
       </c>
       <c r="M3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.99665022953534887</v>
       </c>
@@ -5758,7 +5803,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J4" s="2">
         <v>45689</v>
@@ -5770,10 +5815,10 @@
         <v>2025</v>
       </c>
       <c r="M4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.0009030939641459</v>
       </c>
@@ -5799,7 +5844,7 @@
         <v>1.5</v>
       </c>
       <c r="I5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J5" s="2">
         <v>45717</v>
@@ -5811,10 +5856,10 @@
         <v>2025</v>
       </c>
       <c r="M5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.99416296692989137</v>
       </c>
@@ -5840,7 +5885,7 @@
         <v>0.9</v>
       </c>
       <c r="I6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J6" s="2">
         <v>45748</v>
@@ -5852,10 +5897,10 @@
         <v>2025</v>
       </c>
       <c r="M6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.99426838465038325</v>
       </c>
@@ -5881,7 +5926,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J7" s="2">
         <v>45778</v>
@@ -5893,10 +5938,10 @@
         <v>2025</v>
       </c>
       <c r="M7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.99489981218709578</v>
       </c>
@@ -5922,7 +5967,7 @@
         <v>1.2</v>
       </c>
       <c r="I8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J8" s="2">
         <v>45809</v>
@@ -5934,10 +5979,10 @@
         <v>2025</v>
       </c>
       <c r="M8" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.99624089267593119</v>
       </c>
@@ -5963,7 +6008,7 @@
         <v>1.4</v>
       </c>
       <c r="I9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J9" s="2">
         <v>45839</v>
@@ -5975,10 +6020,10 @@
         <v>2025</v>
       </c>
       <c r="M9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.99530785090469787</v>
       </c>
@@ -6004,7 +6049,7 @@
         <v>1.5</v>
       </c>
       <c r="I10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J10" s="2">
         <v>45870</v>
@@ -6016,10 +6061,10 @@
         <v>2025</v>
       </c>
       <c r="M10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.99436522839520647</v>
       </c>
@@ -6045,7 +6090,7 @@
         <v>1.5</v>
       </c>
       <c r="I11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J11" s="2">
         <v>45901</v>
@@ -6057,10 +6102,10 @@
         <v>2025</v>
       </c>
       <c r="M11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.99369858073286665</v>
       </c>
@@ -6086,7 +6131,7 @@
         <v>1.6</v>
       </c>
       <c r="I12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J12" s="2">
         <v>45931</v>
@@ -6098,10 +6143,10 @@
         <v>2025</v>
       </c>
       <c r="M12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.99206581450654974</v>
       </c>
@@ -6127,7 +6172,7 @@
         <v>1.6</v>
       </c>
       <c r="I13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J13" s="2">
         <v>45962</v>
@@ -6139,7 +6184,89 @@
         <v>2025</v>
       </c>
       <c r="M13" t="s">
-        <v>201</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.99337421677880722</v>
+      </c>
+      <c r="B14">
+        <v>-0.66257832211927825</v>
+      </c>
+      <c r="C14">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>12.706424505276701</v>
+      </c>
+      <c r="E14">
+        <v>4.0691604975969771</v>
+      </c>
+      <c r="F14">
+        <v>1.1415452718598471</v>
+      </c>
+      <c r="G14">
+        <v>-3.1</v>
+      </c>
+      <c r="H14">
+        <v>1.7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>212</v>
+      </c>
+      <c r="J14" s="2">
+        <v>45992</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>2025</v>
+      </c>
+      <c r="M14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.9949962127520966</v>
+      </c>
+      <c r="B15">
+        <v>-0.50037872479034018</v>
+      </c>
+      <c r="C15">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>12.407063707315929</v>
+      </c>
+      <c r="E15">
+        <v>2.9087958171008061</v>
+      </c>
+      <c r="F15">
+        <v>0.82580732520625832</v>
+      </c>
+      <c r="G15">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="H15">
+        <v>1.2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>213</v>
+      </c>
+      <c r="J15" s="2">
+        <v>45992</v>
+      </c>
+      <c r="K15">
+        <v>12</v>
+      </c>
+      <c r="L15">
+        <v>2025</v>
+      </c>
+      <c r="M15" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>